<commit_message>
Apparently CSV's are bad
</commit_message>
<xml_diff>
--- a/Logs/Analysis/Master.xlsx
+++ b/Logs/Analysis/Master.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="15940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Subject</t>
   </si>
@@ -51,6 +51,15 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Constant</t>
+  </si>
+  <si>
+    <t>Ramp</t>
+  </si>
+  <si>
+    <t>Exponential</t>
   </si>
 </sst>
 </file>
@@ -365,15 +374,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -395,8 +404,17 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -417,6 +435,15 @@
       </c>
       <c r="G2">
         <v>4141.5302600000005</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Master through 5 analysis
</commit_message>
<xml_diff>
--- a/Logs/Analysis/Master.xlsx
+++ b/Logs/Analysis/Master.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="15940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -374,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -469,6 +469,75 @@
         <v>4774.6919600000001</v>
       </c>
     </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3138.68957</v>
+      </c>
+      <c r="C4">
+        <v>5478.2784000000001</v>
+      </c>
+      <c r="D4">
+        <v>3089.7271700000001</v>
+      </c>
+      <c r="E4">
+        <v>5217.8147600000002</v>
+      </c>
+      <c r="F4">
+        <v>9750.6852500000005</v>
+      </c>
+      <c r="G4">
+        <v>6987.0085499999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>3280.2857600000002</v>
+      </c>
+      <c r="C5">
+        <v>2887.8405699999998</v>
+      </c>
+      <c r="D5">
+        <v>2336.8552199999999</v>
+      </c>
+      <c r="E5">
+        <v>3256.7347799999998</v>
+      </c>
+      <c r="F5">
+        <v>2735.1353399999998</v>
+      </c>
+      <c r="G5">
+        <v>2958.6165000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>8844.9357299999992</v>
+      </c>
+      <c r="C6">
+        <v>3560.35734</v>
+      </c>
+      <c r="D6">
+        <v>9405.7161099999994</v>
+      </c>
+      <c r="E6">
+        <v>6366.9946600000003</v>
+      </c>
+      <c r="F6">
+        <v>6870.6650900000004</v>
+      </c>
+      <c r="G6">
+        <v>6293.7765200000003</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Master through 6 analysis
</commit_message>
<xml_diff>
--- a/Logs/Analysis/Master.xlsx
+++ b/Logs/Analysis/Master.xlsx
@@ -374,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -538,6 +538,29 @@
         <v>6293.7765200000003</v>
       </c>
     </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2724.6348400000002</v>
+      </c>
+      <c r="C7">
+        <v>5406.0033199999998</v>
+      </c>
+      <c r="D7">
+        <v>5139.5067499999996</v>
+      </c>
+      <c r="E7">
+        <v>8878.2346699999998</v>
+      </c>
+      <c r="F7">
+        <v>4469.6042699999998</v>
+      </c>
+      <c r="G7">
+        <v>11283.687599999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>